<commit_message>
diapo et correction rapport
</commit_message>
<xml_diff>
--- a/Rapport/bd.xlsx
+++ b/Rapport/bd.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\EasyPHP-Devserver-17\eds-www\Casier-Connecte\Rapport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E3C3129-E9AA-4686-9E59-F4283E25D884}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AB4D045-F9DA-4A13-BA09-42CF238E1BF4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DCC55444-8661-40C8-8DE7-22DC22BCA2FB}"/>
+    <workbookView xWindow="-28920" yWindow="-2370" windowWidth="29040" windowHeight="15840" xr2:uid="{DCC55444-8661-40C8-8DE7-22DC22BCA2FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -586,7 +586,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -610,13 +610,6 @@
     </font>
     <font>
       <b/>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -895,6 +888,15 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -931,21 +933,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -958,12 +951,178 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="9"/>
+        <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1000,172 +1159,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1180,14 +1173,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2417472E-5F54-4BEA-8F27-2210D9B51AB6}" name="Tableau1" displayName="Tableau1" ref="K1:O51" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" headerRowBorderDxfId="8" tableBorderDxfId="9" totalsRowBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2417472E-5F54-4BEA-8F27-2210D9B51AB6}" name="Tableau1" displayName="Tableau1" ref="K1:O51" totalsRowShown="0" headerRowDxfId="9" dataDxfId="0" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
   <autoFilter ref="K1:O51" xr:uid="{9AE526E6-98A0-4667-83B3-0B691EDA856E}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{59A679C1-3F66-4C76-B1C0-2EC44B811EDE}" name="Code" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{46E654ED-E166-42F7-888D-E607AC548942}" name="Description" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{E3511C77-8726-43D3-BA90-37412B2AB364}" name="Type" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{2CE3EB6C-AA38-4212-A2E1-C525169071B6}" name="Format" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{6AEED1C3-25C2-4A67-998D-D506624FB51C}" name="Régle" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{59A679C1-3F66-4C76-B1C0-2EC44B811EDE}" name="Code" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{46E654ED-E166-42F7-888D-E607AC548942}" name="Description" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{E3511C77-8726-43D3-BA90-37412B2AB364}" name="Type" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{2CE3EB6C-AA38-4212-A2E1-C525169071B6}" name="Format" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{6AEED1C3-25C2-4A67-998D-D506624FB51C}" name="Régle" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1492,8 +1485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71B160F2-6F42-409A-9C44-E2FBB7997183}">
   <dimension ref="A1:O55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L54" sqref="L54"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1510,13 +1503,13 @@
     <col min="11" max="11" width="20.85546875" customWidth="1"/>
     <col min="12" max="12" width="33.5703125" customWidth="1"/>
     <col min="13" max="13" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.140625" customWidth="1"/>
-    <col min="15" max="15" width="13.5703125" customWidth="1"/>
+    <col min="14" max="14" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="37.28515625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="40" t="s">
         <v>76</v>
       </c>
       <c r="B1" s="26" t="s">
@@ -1535,24 +1528,24 @@
         <v>52</v>
       </c>
       <c r="G1" s="36"/>
-      <c r="K1" s="49" t="s">
+      <c r="K1" s="37" t="s">
         <v>120</v>
       </c>
-      <c r="L1" s="50" t="s">
+      <c r="L1" s="38" t="s">
         <v>119</v>
       </c>
-      <c r="M1" s="50" t="s">
+      <c r="M1" s="38" t="s">
         <v>121</v>
       </c>
-      <c r="N1" s="50" t="s">
+      <c r="N1" s="38" t="s">
         <v>123</v>
       </c>
-      <c r="O1" s="51" t="s">
+      <c r="O1" s="39" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="38"/>
+      <c r="A2" s="41"/>
       <c r="B2" s="24" t="s">
         <v>0</v>
       </c>
@@ -1586,7 +1579,7 @@
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="38"/>
+      <c r="A3" s="41"/>
       <c r="B3" s="24" t="s">
         <v>1</v>
       </c>
@@ -1618,7 +1611,7 @@
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="38"/>
+      <c r="A4" s="41"/>
       <c r="B4" s="24" t="s">
         <v>2</v>
       </c>
@@ -1644,7 +1637,7 @@
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="38"/>
+      <c r="A5" s="41"/>
       <c r="B5" s="24" t="s">
         <v>3</v>
       </c>
@@ -1670,7 +1663,7 @@
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="39"/>
+      <c r="A6" s="42"/>
       <c r="B6" s="25" t="s">
         <v>19</v>
       </c>
@@ -1744,7 +1737,7 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="40" t="s">
+      <c r="A9" s="43" t="s">
         <v>74</v>
       </c>
       <c r="B9" s="30" t="s">
@@ -1782,7 +1775,7 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="41"/>
+      <c r="A10" s="44"/>
       <c r="B10" s="28" t="s">
         <v>10</v>
       </c>
@@ -1818,7 +1811,7 @@
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="42"/>
+      <c r="A11" s="45"/>
       <c r="B11" s="29"/>
       <c r="C11" s="12" t="s">
         <v>49</v>
@@ -1896,7 +1889,7 @@
       <c r="O13" s="54"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="43" t="s">
+      <c r="A14" s="46" t="s">
         <v>77</v>
       </c>
       <c r="B14" s="20" t="s">
@@ -1932,7 +1925,7 @@
       <c r="O14" s="54"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="44"/>
+      <c r="A15" s="47"/>
       <c r="B15" s="21" t="s">
         <v>28</v>
       </c>
@@ -1966,7 +1959,7 @@
       <c r="O15" s="54"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="44"/>
+      <c r="A16" s="47"/>
       <c r="B16" s="21" t="s">
         <v>51</v>
       </c>
@@ -1998,7 +1991,7 @@
       <c r="O16" s="54"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="44"/>
+      <c r="A17" s="47"/>
       <c r="B17" s="21"/>
       <c r="C17" s="6" t="s">
         <v>22</v>
@@ -2024,7 +2017,7 @@
       <c r="O17" s="54"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="44"/>
+      <c r="A18" s="47"/>
       <c r="B18" s="21"/>
       <c r="C18" s="6"/>
       <c r="D18" s="21"/>
@@ -2048,7 +2041,7 @@
       <c r="O18" s="54"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="44"/>
+      <c r="A19" s="47"/>
       <c r="B19" s="21"/>
       <c r="C19" s="6"/>
       <c r="D19" s="21"/>
@@ -2072,7 +2065,7 @@
       <c r="O19" s="54"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="44"/>
+      <c r="A20" s="47"/>
       <c r="B20" s="21"/>
       <c r="C20" s="6"/>
       <c r="D20" s="21"/>
@@ -2098,7 +2091,7 @@
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="44"/>
+      <c r="A21" s="47"/>
       <c r="B21" s="21"/>
       <c r="C21" s="6"/>
       <c r="D21" s="21"/>
@@ -2124,7 +2117,7 @@
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="45"/>
+      <c r="A22" s="48"/>
       <c r="B22" s="22"/>
       <c r="C22" s="8"/>
       <c r="D22" s="22"/>
@@ -2196,7 +2189,7 @@
       <c r="O24" s="54"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="46" t="s">
+      <c r="A25" s="49" t="s">
         <v>75</v>
       </c>
       <c r="B25" s="33" t="s">
@@ -2232,7 +2225,7 @@
       <c r="O25" s="54"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26" s="47"/>
+      <c r="A26" s="50"/>
       <c r="B26" s="34" t="s">
         <v>10</v>
       </c>
@@ -2266,7 +2259,7 @@
       <c r="O26" s="54"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="47"/>
+      <c r="A27" s="50"/>
       <c r="B27" s="34" t="s">
         <v>7</v>
       </c>
@@ -2300,7 +2293,7 @@
       <c r="O27" s="54"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A28" s="47"/>
+      <c r="A28" s="50"/>
       <c r="B28" s="34"/>
       <c r="C28" s="1" t="s">
         <v>10</v>
@@ -2334,7 +2327,7 @@
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29" s="47"/>
+      <c r="A29" s="50"/>
       <c r="B29" s="34"/>
       <c r="C29" s="1"/>
       <c r="D29" s="34"/>
@@ -2358,7 +2351,7 @@
       <c r="O29" s="54"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="47"/>
+      <c r="A30" s="50"/>
       <c r="B30" s="34"/>
       <c r="C30" s="1"/>
       <c r="D30" s="34"/>
@@ -2382,7 +2375,7 @@
       <c r="O30" s="54"/>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="47"/>
+      <c r="A31" s="50"/>
       <c r="B31" s="34"/>
       <c r="C31" s="1"/>
       <c r="D31" s="34"/>
@@ -2404,7 +2397,7 @@
       <c r="O31" s="54"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="47"/>
+      <c r="A32" s="50"/>
       <c r="B32" s="33" t="s">
         <v>26</v>
       </c>
@@ -2440,7 +2433,7 @@
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A33" s="47"/>
+      <c r="A33" s="50"/>
       <c r="B33" s="34" t="s">
         <v>31</v>
       </c>
@@ -2474,7 +2467,7 @@
       <c r="O33" s="54"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A34" s="47"/>
+      <c r="A34" s="50"/>
       <c r="B34" s="34"/>
       <c r="C34" s="1" t="s">
         <v>19</v>
@@ -2506,7 +2499,7 @@
       <c r="O34" s="54"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A35" s="47"/>
+      <c r="A35" s="50"/>
       <c r="B35" s="34" t="s">
         <v>10</v>
       </c>
@@ -2536,7 +2529,7 @@
       <c r="O35" s="54"/>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A36" s="47"/>
+      <c r="A36" s="50"/>
       <c r="B36" s="34" t="s">
         <v>27</v>
       </c>
@@ -2566,7 +2559,7 @@
       <c r="O36" s="54"/>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A37" s="47"/>
+      <c r="A37" s="50"/>
       <c r="B37" s="34" t="s">
         <v>16</v>
       </c>
@@ -2592,7 +2585,7 @@
       <c r="O37" s="54"/>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A38" s="47"/>
+      <c r="A38" s="50"/>
       <c r="B38" s="34"/>
       <c r="C38" s="1"/>
       <c r="D38" s="34"/>
@@ -2618,7 +2611,7 @@
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A39" s="47"/>
+      <c r="A39" s="50"/>
       <c r="B39" s="34"/>
       <c r="C39" s="1"/>
       <c r="D39" s="34"/>
@@ -2642,7 +2635,7 @@
       <c r="O39" s="54"/>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A40" s="48"/>
+      <c r="A40" s="51"/>
       <c r="B40" s="35"/>
       <c r="C40" s="4"/>
       <c r="D40" s="35"/>

</xml_diff>